<commit_message>
Added basecount to results
</commit_message>
<xml_diff>
--- a/Filter_Usecase/Results_no_indels_new_t0_new_decision_tree.xlsx
+++ b/Filter_Usecase/Results_no_indels_new_t0_new_decision_tree.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\volume1\ido\BN-SCRIPTS\Filter_Usecase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BE4750DE-6AD2-4842-B7CA-F3CB73C111D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DA2A6-EFD8-42F0-BDAC-1705DD083C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3855" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-28920" yWindow="-2400" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$I$47</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Patient</t>
   </si>
@@ -78,11 +91,14 @@
   <si>
     <t>P6</t>
   </si>
+  <si>
+    <t>N9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -655,6 +671,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -700,28 +729,31 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1096,11 +1128,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1108,7 +1140,7 @@
     <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
@@ -1147,36 +1179,36 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>741140288</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>44627</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>26</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>88512</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>2</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>1446</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>87064</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="2">
         <v>45</v>
       </c>
@@ -1198,12 +1230,12 @@
       <c r="H3" s="2">
         <v>1510</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>86994</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="2">
         <v>165</v>
       </c>
@@ -1225,12 +1257,12 @@
       <c r="H4" s="2">
         <v>13146</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <v>75331</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="2">
         <v>189</v>
       </c>
@@ -1252,124 +1284,124 @@
       <c r="H5" s="2">
         <v>14215</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>74262</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12">
+      <c r="A6" s="14"/>
+      <c r="B6" s="9">
         <v>241</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>741299538</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="10">
         <v>44868</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>27.4</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="9">
         <v>88512</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="9">
         <v>32</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>11238</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="11">
         <v>77242</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>741286954</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>44727</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>23.37</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>88050</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>6</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>3339</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>84705</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12">
+      <c r="A8" s="14"/>
+      <c r="B8" s="9">
         <v>14</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <v>741288907</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <v>44741</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="9">
         <v>30.83</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="9">
         <v>88050</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="9">
         <v>0</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="9">
         <v>12983</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="11">
         <v>75067</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>741148584</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>44662</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>30</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>88545</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>2</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>13270</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>75273</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="2">
         <v>5</v>
       </c>
@@ -1391,12 +1423,12 @@
       <c r="H10" s="2">
         <v>204</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="8">
         <v>88322</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2">
         <v>30</v>
       </c>
@@ -1418,124 +1450,124 @@
       <c r="H11" s="2">
         <v>5333</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="8">
         <v>83207</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12">
+      <c r="A12" s="14"/>
+      <c r="B12" s="9">
         <v>76</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <v>741288510</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="10">
         <v>44738</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>27.5</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="9">
         <v>88545</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="9">
         <v>14</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="9">
         <v>4820</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="11">
         <v>83711</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>0</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>741149041</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>44665</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>18.62</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>87783</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>2</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>617</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>87164</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12">
+      <c r="A14" s="14"/>
+      <c r="B14" s="9">
         <v>27</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="9">
         <v>741284247</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <v>44692</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>26.73</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="9">
         <v>87783</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="9">
         <v>3</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="9">
         <v>2059</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="11">
         <v>85721</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>0</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>741146626</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>44652</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>26.5</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>88551</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>4</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>1098</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>87449</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="2">
         <v>13</v>
       </c>
@@ -1557,12 +1589,12 @@
       <c r="H16" s="2">
         <v>149</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="8">
         <v>88368</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="2">
         <v>16</v>
       </c>
@@ -1584,12 +1616,12 @@
       <c r="H17" s="2">
         <v>3682</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <v>84841</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="2">
         <v>19</v>
       </c>
@@ -1611,12 +1643,12 @@
       <c r="H18" s="2">
         <v>4775</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="8">
         <v>83770</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="2">
         <v>23</v>
       </c>
@@ -1638,12 +1670,12 @@
       <c r="H19" s="2">
         <v>2005</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="8">
         <v>86527</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="2">
         <v>26</v>
       </c>
@@ -1665,12 +1697,12 @@
       <c r="H20" s="2">
         <v>286</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="8">
         <v>88247</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="2">
         <v>31</v>
       </c>
@@ -1692,178 +1724,180 @@
       <c r="H21" s="2">
         <v>151</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="8">
         <v>88374</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
-      <c r="B22" s="2">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="13"/>
+      <c r="B22" s="15">
         <v>37</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="15">
         <v>741283709</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="16">
         <v>44689</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="15">
         <v>34</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="15">
         <v>88551</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="15">
         <v>5</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="15">
         <v>2945</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="17">
         <v>85601</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
-      <c r="B23" s="2">
+      <c r="A23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5">
         <v>0</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="5">
         <v>741302132</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="6">
         <v>44904</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="5">
         <v>23</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="5">
         <v>88503</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="5">
         <v>1</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="5">
         <v>939</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="7">
         <v>87563</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12">
+      <c r="A24" s="14"/>
+      <c r="B24" s="9">
         <v>26</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="9">
         <v>741304163</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="10">
         <v>44930</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="9">
         <v>18.5</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="9">
         <v>88503</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="9">
         <v>0</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="9">
         <v>26021</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="11">
         <v>62482</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>0</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>740665529</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>44228</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>14.07</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>87987</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>14</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <v>5687</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="7">
         <v>82286</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12">
+      <c r="A26" s="14"/>
+      <c r="B26" s="9">
         <v>16</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="9">
         <v>740656183</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="10">
         <v>44244</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="9">
         <v>27.43</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="9">
         <v>87987</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="9">
         <v>1</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="9">
         <v>382</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="11">
         <v>87604</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>0</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>740652926</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>44223</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>21.47</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>88566</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>3</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <v>37</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="7">
         <v>88526</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="2">
         <v>10</v>
       </c>
@@ -1885,12 +1919,12 @@
       <c r="H28" s="2">
         <v>6124</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="8">
         <v>82435</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="2">
         <v>13</v>
       </c>
@@ -1912,12 +1946,12 @@
       <c r="H29" s="2">
         <v>20657</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="8">
         <v>67907</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="2">
         <v>18</v>
       </c>
@@ -1939,12 +1973,12 @@
       <c r="H30" s="2">
         <v>6635</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="8">
         <v>81927</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="2">
         <v>25</v>
       </c>
@@ -1966,12 +2000,12 @@
       <c r="H31" s="2">
         <v>6636</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="8">
         <v>81928</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="2">
         <v>28</v>
       </c>
@@ -1993,68 +2027,68 @@
       <c r="H32" s="2">
         <v>11510</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="8">
         <v>77051</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12">
+      <c r="A33" s="14"/>
+      <c r="B33" s="9">
         <v>35</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="9">
         <v>740671764</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="10">
         <v>44258</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="9">
         <v>30.5</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="9">
         <v>88566</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="9">
         <v>1</v>
       </c>
-      <c r="H33" s="12">
+      <c r="H33" s="9">
         <v>9962</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I33" s="11">
         <v>78603</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>0</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>740605134</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>44475</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <v>22.5</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5">
         <v>88692</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="5">
         <v>12</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="5">
         <v>2781</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I34" s="7">
         <v>85899</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="9"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="2">
         <v>12</v>
       </c>
@@ -2076,12 +2110,12 @@
       <c r="H35" s="2">
         <v>37</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="8">
         <v>88647</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="9"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="2">
         <v>20</v>
       </c>
@@ -2103,12 +2137,12 @@
       <c r="H36" s="2">
         <v>6805</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="8">
         <v>81875</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="9"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="2">
         <v>27</v>
       </c>
@@ -2130,12 +2164,12 @@
       <c r="H37" s="2">
         <v>20454</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="8">
         <v>68236</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="9"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="2">
         <v>30</v>
       </c>
@@ -2157,12 +2191,12 @@
       <c r="H38" s="2">
         <v>34</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="8">
         <v>88647</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="9"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="2">
         <v>40</v>
       </c>
@@ -2184,12 +2218,12 @@
       <c r="H39" s="2">
         <v>1807</v>
       </c>
-      <c r="I39" s="10">
+      <c r="I39" s="8">
         <v>86871</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="9"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="2">
         <v>44</v>
       </c>
@@ -2211,12 +2245,12 @@
       <c r="H40" s="2">
         <v>9249</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I40" s="8">
         <v>79431</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="2">
         <v>68</v>
       </c>
@@ -2238,68 +2272,68 @@
       <c r="H41" s="2">
         <v>703</v>
       </c>
-      <c r="I41" s="10">
+      <c r="I41" s="8">
         <v>87971</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="11"/>
-      <c r="B42" s="12">
+      <c r="A42" s="14"/>
+      <c r="B42" s="9">
         <v>75</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="9">
         <v>740628355</v>
       </c>
-      <c r="D42" s="13">
+      <c r="D42" s="10">
         <v>44550</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="9">
         <v>28</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42" s="9">
         <v>88692</v>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="9">
         <v>14</v>
       </c>
-      <c r="H42" s="12">
+      <c r="H42" s="9">
         <v>10783</v>
       </c>
-      <c r="I42" s="14">
+      <c r="I42" s="11">
         <v>77895</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <v>0</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <v>740626783</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="6">
         <v>44181</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <v>17</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="5">
         <v>88695</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="5">
         <v>2</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H43" s="5">
         <v>894</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I43" s="7">
         <v>87799</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="9"/>
+      <c r="A44" s="13"/>
       <c r="B44" s="2">
         <v>22</v>
       </c>
@@ -2321,12 +2355,12 @@
       <c r="H44" s="2">
         <v>18</v>
       </c>
-      <c r="I44" s="10">
+      <c r="I44" s="8">
         <v>88669</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="9"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="2">
         <v>30</v>
       </c>
@@ -2348,12 +2382,12 @@
       <c r="H45" s="2">
         <v>1717</v>
       </c>
-      <c r="I45" s="10">
+      <c r="I45" s="8">
         <v>86975</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="9"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="2">
         <v>35</v>
       </c>
@@ -2375,40 +2409,40 @@
       <c r="H46" s="2">
         <v>533</v>
       </c>
-      <c r="I46" s="10">
+      <c r="I46" s="8">
         <v>88134</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="11"/>
-      <c r="B47" s="12">
+      <c r="A47" s="14"/>
+      <c r="B47" s="9">
         <v>37</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47" s="9">
         <v>740650265</v>
       </c>
-      <c r="D47" s="13">
+      <c r="D47" s="10">
         <v>44218</v>
       </c>
-      <c r="E47" s="12">
+      <c r="E47" s="9">
         <v>27</v>
       </c>
-      <c r="F47" s="12">
+      <c r="F47" s="9">
         <v>88695</v>
       </c>
-      <c r="G47" s="12">
+      <c r="G47" s="9">
         <v>4</v>
       </c>
-      <c r="H47" s="12">
+      <c r="H47" s="9">
         <v>585</v>
       </c>
-      <c r="I47" s="14">
+      <c r="I47" s="11">
         <v>88106</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I47"/>
-  <mergeCells count="9">
+  <autoFilter ref="A1:I47" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="10">
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A2:A6"/>
@@ -2416,9 +2450,11 @@
     <mergeCell ref="A34:A42"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A15:A24"/>
     <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>